<commit_message>
agregado de password en import xlsx
</commit_message>
<xml_diff>
--- a/backend/templates/plantilla-importacion-clientes-vehiculos.xlsx
+++ b/backend/templates/plantilla-importacion-clientes-vehiculos.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,12 +439,12 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>- address: Dirección completa (obligatorio)</v>
+        <v>- address: Dirección completa (opcional)</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>- notes: Notas adicionales (opcional)</v>
+        <v>- password: Contraseña del cliente (obligatorio)</v>
       </c>
     </row>
     <row r="9">
@@ -509,27 +509,42 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>- Los emails deben ser únicos y válidos</v>
+        <v>- Campos obligatorios para clientes: name, email, phone, password</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>- Las placas deben ser únicas</v>
+        <v>- Campo opcional para clientes: address (puede dejarse vacío)</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>- El año debe ser un número válido</v>
+        <v>- Los emails deben ser únicos y válidos</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
+        <v>- Las placas deben ser únicas</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>- El año debe ser un número válido</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>- Las contraseñas se almacenarán tal como se escriban</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
         <v>- Asegúrese de que el email del cliente existe antes de asignar vehículos</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A27"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -545,7 +560,7 @@
     <col min="2" max="2" customWidth="1" width="30"/>
     <col min="3" max="3" customWidth="1" width="15"/>
     <col min="4" max="4" customWidth="1" width="40"/>
-    <col min="5" max="5" customWidth="1" width="30"/>
+    <col min="5" max="5" customWidth="1" width="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -562,7 +577,7 @@
         <v>address</v>
       </c>
       <c r="E1" t="str">
-        <v>notes</v>
+        <v>password</v>
       </c>
     </row>
     <row r="2">
@@ -579,7 +594,7 @@
         <v>Col. Centro, Calle 5 #123</v>
       </c>
       <c r="E2" t="str">
-        <v>Cliente frecuente</v>
+        <v>mipassword123</v>
       </c>
     </row>
     <row r="3">
@@ -596,7 +611,7 @@
         <v>Barrio Norte, Av. Principal #456</v>
       </c>
       <c r="E3" t="str">
-        <v>Requiere servicios especializados</v>
+        <v>password456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>